<commit_message>
helcom & de bailly handlers
</commit_message>
<xml_diff>
--- a/nbs/files/lut/dbo_nuclide.xlsx
+++ b/nbs/files/lut/dbo_nuclide.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25930"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iaeacloud-my.sharepoint.com/personal/c_omata_iaea_org/Documents/Desktop/dbo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7156ED16-9DA3-4746-8817-0046D74DDA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{10F122F4-37E7-419D-A9CD-F520E8375053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-26430" yWindow="2130" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -233,7 +233,7 @@
     <t>106mAg</t>
   </si>
   <si>
-    <t>mag106</t>
+    <t>ag106m</t>
   </si>
   <si>
     <t>108Ag</t>
@@ -248,13 +248,13 @@
     <t>108mAg</t>
   </si>
   <si>
-    <t>mag108</t>
+    <t>ag108m</t>
   </si>
   <si>
     <t>110mAg</t>
   </si>
   <si>
-    <t>mag110</t>
+    <t>ag110m</t>
   </si>
   <si>
     <t>ANTIMONY</t>
@@ -278,7 +278,7 @@
     <t>129mTe</t>
   </si>
   <si>
-    <t>mte129</t>
+    <t>te129m</t>
   </si>
   <si>
     <t>IODINE</t>
@@ -725,7 +725,7 @@
     <t>192Ir</t>
   </si>
   <si>
-    <t>lr192</t>
+    <t>ir192</t>
   </si>
   <si>
     <t>238,240Pu</t>
@@ -764,7 +764,7 @@
     <t>117mSn</t>
   </si>
   <si>
-    <t>msn117</t>
+    <t>sn117m</t>
   </si>
   <si>
     <t>THALLIUM</t>
@@ -773,7 +773,7 @@
     <t>208Tl</t>
   </si>
   <si>
-    <t>ti208</t>
+    <t>tl208</t>
   </si>
   <si>
     <t>MOLYBDENUM</t>
@@ -788,7 +788,7 @@
     <t>99mTc</t>
   </si>
   <si>
-    <t>mtc99</t>
+    <t>tc99m</t>
   </si>
   <si>
     <t>105Ru</t>
@@ -884,13 +884,13 @@
     <t>116mIn</t>
   </si>
   <si>
-    <t>min116</t>
+    <t>in116m</t>
   </si>
   <si>
     <t>123mTe</t>
   </si>
   <si>
-    <t>mte123</t>
+    <t>te123m</t>
   </si>
   <si>
     <t>127Sb</t>
@@ -938,7 +938,7 @@
     <t>234mPa</t>
   </si>
   <si>
-    <t>mpa234</t>
+    <t>pa234m</t>
   </si>
   <si>
     <t>243Am</t>
@@ -998,7 +998,7 @@
     <t>137mBa</t>
   </si>
   <si>
-    <t>mba137</t>
+    <t>ba137m</t>
   </si>
   <si>
     <t>232U</t>
@@ -1907,8 +1907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="H79" sqref="H79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5415,15 +5415,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006C266C02A97D1D41B60FC5BB4AB3B561" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="627c5da731661f4bf76604184727f2d6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f3c01d95-e195-4940-9fb4-afa395d98e0b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6bf665a11c7ceb3b31f5a9dbdfc3fcda" ns2:_="">
     <xsd:import namespace="f3c01d95-e195-4940-9fb4-afa395d98e0b"/>
@@ -5555,14 +5546,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CAE12FE-F927-4AED-AF5B-6EFB75744B94}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C0E32B0-2BF7-4F1D-96E1-B5E1D973E33F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E33F4B43-F626-4BCA-B49E-D17CB2B809C6}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E33F4B43-F626-4BCA-B49E-D17CB2B809C6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C0E32B0-2BF7-4F1D-96E1-B5E1D973E33F}"/>
 </file>
</xml_diff>

<commit_message>
fix type of massnb of nuclides name
</commit_message>
<xml_diff>
--- a/nbs/files/lut/dbo_nuclide.xlsx
+++ b/nbs/files/lut/dbo_nuclide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franckalbinet/pro/IAEA/MARIS/marisco/nbs/files/lut/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022C668B-9828-3B4A-A76A-9827B92B0960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768F32A8-DF8E-6D48-9627-D5D6E4AC4581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1067,7 +1067,7 @@
     <t>pu241_pu239_ratio</t>
   </si>
   <si>
-    <t>Not applicable</t>
+    <t>NOT APPLICABLE</t>
   </si>
 </sst>
 </file>
@@ -1911,7 +1911,7 @@
   <dimension ref="A1:H135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5420,6 +5420,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006C266C02A97D1D41B60FC5BB4AB3B561" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="627c5da731661f4bf76604184727f2d6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f3c01d95-e195-4940-9fb4-afa395d98e0b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6bf665a11c7ceb3b31f5a9dbdfc3fcda" ns2:_="">
     <xsd:import namespace="f3c01d95-e195-4940-9fb4-afa395d98e0b"/>
@@ -5551,12 +5557,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5567,6 +5567,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CAE12FE-F927-4AED-AF5B-6EFB75744B94}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E33F4B43-F626-4BCA-B49E-D17CB2B809C6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5584,15 +5593,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CAE12FE-F927-4AED-AF5B-6EFB75744B94}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C0E32B0-2BF7-4F1D-96E1-B5E1D973E33F}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
refactor (wip) to netcdf long format
</commit_message>
<xml_diff>
--- a/nbs/files/lut/dbo_nuclide.xlsx
+++ b/nbs/files/lut/dbo_nuclide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franckalbinet/pro/IAEA/MARIS/marisco/nbs/files/lut/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768F32A8-DF8E-6D48-9627-D5D6E4AC4581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC2936B-45DF-8241-A208-44D9C11D6D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="344">
   <si>
     <t>nuclide_id</t>
   </si>
@@ -1910,8 +1910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H135"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1957,6 +1957,9 @@
       <c r="B2" t="s">
         <v>343</v>
       </c>
+      <c r="H2" t="s">
+        <v>343</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -1979,6 +1982,9 @@
       </c>
       <c r="G3" t="s">
         <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -5426,6 +5432,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006C266C02A97D1D41B60FC5BB4AB3B561" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="627c5da731661f4bf76604184727f2d6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f3c01d95-e195-4940-9fb4-afa395d98e0b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6bf665a11c7ceb3b31f5a9dbdfc3fcda" ns2:_="">
     <xsd:import namespace="f3c01d95-e195-4940-9fb4-afa395d98e0b"/>
@@ -5557,15 +5572,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CAE12FE-F927-4AED-AF5B-6EFB75744B94}">
   <ds:schemaRefs>
@@ -5576,6 +5582,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C0E32B0-2BF7-4F1D-96E1-B5E1D973E33F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E33F4B43-F626-4BCA-B49E-D17CB2B809C6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5591,12 +5605,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C0E32B0-2BF7-4F1D-96E1-B5E1D973E33F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
geotraces handler fixed and encoded as long
</commit_message>
<xml_diff>
--- a/nbs/files/lut/dbo_nuclide.xlsx
+++ b/nbs/files/lut/dbo_nuclide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franckalbinet/pro/IAEA/MARIS/marisco/nbs/files/lut/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC2936B-45DF-8241-A208-44D9C11D6D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D05C5FE-BF49-BE40-BB14-6C6291456200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10840" yWindow="500" windowWidth="17960" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020-05-14 dbo_nuclide" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="349">
   <si>
     <t>nuclide_id</t>
   </si>
@@ -1061,13 +1061,28 @@
     <t>pu240_pu239_ratio</t>
   </si>
   <si>
-    <t>241Pu/239Pu</t>
-  </si>
-  <si>
-    <t>pu241_pu239_ratio</t>
-  </si>
-  <si>
     <t>NOT APPLICABLE</t>
+  </si>
+  <si>
+    <t>ACTINIIUM</t>
+  </si>
+  <si>
+    <t>U-233</t>
+  </si>
+  <si>
+    <t>u233</t>
+  </si>
+  <si>
+    <t>Pu-239,242</t>
+  </si>
+  <si>
+    <t>pu239_242_tot</t>
+  </si>
+  <si>
+    <t>Ac-227</t>
+  </si>
+  <si>
+    <t>ac227</t>
   </si>
 </sst>
 </file>
@@ -1908,10 +1923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H135"/>
+  <dimension ref="A1:H137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H3"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="C119" sqref="C119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1919,6 +1934,7 @@
     <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.5" customWidth="1"/>
     <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" customWidth="1"/>
     <col min="8" max="8" width="23.6640625" bestFit="1" customWidth="1"/>
@@ -1955,10 +1971,10 @@
         <v>-1</v>
       </c>
       <c r="B2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -5398,25 +5414,77 @@
         <v>142</v>
       </c>
       <c r="B135" t="s">
-        <v>208</v>
+        <v>161</v>
       </c>
       <c r="C135">
+        <v>92</v>
+      </c>
+      <c r="D135">
+        <v>233</v>
+      </c>
+      <c r="E135" t="s">
+        <v>343</v>
+      </c>
+      <c r="F135">
+        <v>5021000000000</v>
+      </c>
+      <c r="G135" t="s">
+        <v>61</v>
+      </c>
+      <c r="H135" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>143</v>
+      </c>
+      <c r="B136" t="s">
+        <v>197</v>
+      </c>
+      <c r="C136">
         <v>94</v>
       </c>
-      <c r="D135">
-        <v>241</v>
-      </c>
-      <c r="E135" t="s">
-        <v>341</v>
-      </c>
-      <c r="F135">
-        <v>0</v>
-      </c>
-      <c r="G135" t="s">
+      <c r="D136">
+        <v>239</v>
+      </c>
+      <c r="E136" t="s">
+        <v>345</v>
+      </c>
+      <c r="F136">
+        <v>0</v>
+      </c>
+      <c r="G136" t="s">
         <v>9</v>
       </c>
-      <c r="H135" t="s">
+      <c r="H136" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>144</v>
+      </c>
+      <c r="B137" t="s">
         <v>342</v>
+      </c>
+      <c r="C137">
+        <v>89</v>
+      </c>
+      <c r="D137">
+        <v>227</v>
+      </c>
+      <c r="E137" t="s">
+        <v>347</v>
+      </c>
+      <c r="F137">
+        <v>21.771999999999998</v>
+      </c>
+      <c r="G137" t="s">
+        <v>12</v>
+      </c>
+      <c r="H137" t="s">
+        <v>348</v>
       </c>
     </row>
   </sheetData>
@@ -5426,21 +5494,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006C266C02A97D1D41B60FC5BB4AB3B561" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="627c5da731661f4bf76604184727f2d6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f3c01d95-e195-4940-9fb4-afa395d98e0b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6bf665a11c7ceb3b31f5a9dbdfc3fcda" ns2:_="">
     <xsd:import namespace="f3c01d95-e195-4940-9fb4-afa395d98e0b"/>
@@ -5572,24 +5625,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CAE12FE-F927-4AED-AF5B-6EFB75744B94}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C0E32B0-2BF7-4F1D-96E1-B5E1D973E33F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E33F4B43-F626-4BCA-B49E-D17CB2B809C6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5605,4 +5656,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C0E32B0-2BF7-4F1D-96E1-B5E1D973E33F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CAE12FE-F927-4AED-AF5B-6EFB75744B94}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>